<commit_message>
commit with 2 modified files
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2255766-09BF-47CA-8227-EC0D8734DAE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1074DD8-EB8B-4177-931F-4384C4317CB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Илија</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Сотирова</t>
+  </si>
+  <si>
+    <t>Дарко</t>
+  </si>
+  <si>
+    <t>Ристевски</t>
+  </si>
+  <si>
+    <t>Јована</t>
+  </si>
+  <si>
+    <t>Ѓурковска</t>
   </si>
 </sst>
 </file>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,7 +464,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>183051</v>
+        <v>181004</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -470,6 +482,28 @@
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>186037</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>183160</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>